<commit_message>
listo orden de padres en formulario de editar alumno
</commit_message>
<xml_diff>
--- a/public/pre-inscripciones.xlsx
+++ b/public/pre-inscripciones.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>CODIGO</t>
   </si>
@@ -155,16 +155,25 @@
     <t>NIVEL</t>
   </si>
   <si>
+    <t xml:space="preserve">123412342134 </t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
     <t>DONALD TRUMP</t>
   </si>
   <si>
     <t xml:space="preserve">  DONALD TRUMP</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>NINGUNO</t>
+    <t>H</t>
+  </si>
+  <si>
+    <t>TARIJA</t>
+  </si>
+  <si>
+    <t>ARCE</t>
   </si>
   <si>
     <t>2022-11-11</t>
@@ -1058,38 +1067,41 @@
       <c r="A2" s="1">
         <v>492430</v>
       </c>
-      <c r="B2">
-        <v>123412342134</v>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AC2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AD2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AE2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AF2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AJ2">
         <v>1234234</v>

</xml_diff>